<commit_message>
fix version xlx (#930)
</commit_message>
<xml_diff>
--- a/.storybook/public/audits/DataListGroup.xlsx
+++ b/.storybook/public/audits/DataListGroup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/julien_roche_fabernovel_ey_com/Documents/Documents/CNAM Audits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidfyon/Desktop/cnam/design-system-v3/.storybook/public/audits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6793F44-AAE7-480C-B35C-4EFC7DA39372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7467F796-C34D-B143-A2E8-EF7418A78D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="51200" windowHeight="26640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataListGroup" sheetId="2" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>1.0.2</t>
   </si>
   <si>
-    <t>1.0.16</t>
-  </si>
-  <si>
     <t>Nombre de critères conformes</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
   </si>
   <si>
     <t>https://www.w3.org/WAI/WCAG21/Techniques/html/H48</t>
+  </si>
+  <si>
+    <t>1.0.6</t>
   </si>
 </sst>
 </file>
@@ -963,13 +963,11 @@
       <sz val="13.5"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="13.5"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1213,23 +1211,26 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1239,18 +1240,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1276,17 +1265,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1673,162 +1671,162 @@
   <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="115.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="115.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.1" customHeight="1">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="32" customHeight="1">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
-      <c r="A2" s="24" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" ht="19">
+      <c r="A2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
       <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="24" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:6" ht="19">
+      <c r="A3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
       <c r="D3" s="8">
         <v>45855</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="20">
         <v>45761</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:6" ht="19">
+      <c r="A4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1">
+      <c r="A5" s="39" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.95" customHeight="1">
-      <c r="A5" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="9">
         <f xml:space="preserve"> COUNTIF($D$14:$D$119,"Conforme")</f>
         <v>7</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="21">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18.75">
-      <c r="A6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+    <row r="6" spans="1:6" ht="19">
+      <c r="A6" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="9">
         <f xml:space="preserve"> COUNTIF($D$14:$D$119,"Non conforme")</f>
         <v>1</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
-      <c r="A7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+    <row r="7" spans="1:6" ht="19">
+      <c r="A7" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="9">
         <f xml:space="preserve"> COUNTIF($D$14:$D$119,"Non applicable")</f>
         <v>98</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="21">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
-      <c r="A8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
+    <row r="8" spans="1:6" ht="19">
+      <c r="A8" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="9">
         <f xml:space="preserve"> COUNTIF($D$14:$D$119,"Dérogé")</f>
         <v>0</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
-      <c r="A9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+    <row r="9" spans="1:6" ht="19">
+      <c r="A9" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="9">
         <f xml:space="preserve"> COUNTIF($D$14:$D$119,"Non testé")</f>
         <v>0</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="21">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A10" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
+    <row r="10" spans="1:6" ht="19" customHeight="1">
+      <c r="A10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="14">
         <f>IF(SUM(D5:D6)&gt;0,D5/SUM(D5:D6),"")</f>
         <v>0.875</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18.95" customHeight="1">
-      <c r="A11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
+    <row r="11" spans="1:6" ht="19" customHeight="1">
+      <c r="A11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="14">
         <f>IF(SUM(D5:D6)&gt;0,1-ROUND(D10,2),"")</f>
         <v>0.12</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="22">
         <v>0</v>
       </c>
     </row>
@@ -1837,1605 +1835,1618 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="18.95">
+    <row r="13" spans="1:6" ht="19">
       <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="16" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="34">
+      <c r="A14" s="40" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="33.950000000000003">
-      <c r="A14" s="28" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" ht="33.950000000000003">
-      <c r="A15" s="29"/>
+    <row r="15" spans="1:6" ht="34">
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" ht="33.950000000000003">
-      <c r="A16" s="29"/>
+    <row r="16" spans="1:6" ht="34">
+      <c r="A16" s="26"/>
       <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="51">
-      <c r="A17" s="29"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="33.950000000000003">
-      <c r="A18" s="29"/>
+    <row r="18" spans="1:6" ht="34">
+      <c r="A18" s="26"/>
       <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="33.950000000000003">
-      <c r="A19" s="29"/>
+    <row r="19" spans="1:6" ht="34">
+      <c r="A19" s="26"/>
       <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" ht="33.950000000000003">
-      <c r="A20" s="29"/>
+    <row r="20" spans="1:6" ht="34">
+      <c r="A20" s="26"/>
       <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="51">
-      <c r="A21" s="29"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" ht="33.950000000000003">
-      <c r="A22" s="30"/>
+    <row r="22" spans="1:6" ht="34">
+      <c r="A22" s="27"/>
       <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" ht="18.95">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:6" ht="19">
+      <c r="A23" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" ht="33.950000000000003">
-      <c r="A24" s="30"/>
+    <row r="24" spans="1:6" ht="34">
+      <c r="A24" s="27"/>
       <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="33.950000000000003">
-      <c r="A25" s="31" t="s">
+    <row r="25" spans="1:6" ht="34">
+      <c r="A25" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" ht="51">
-      <c r="A26" s="29"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6" ht="51">
-      <c r="A27" s="30"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" ht="33.950000000000003">
-      <c r="A28" s="31" t="s">
+    <row r="28" spans="1:6" ht="34">
+      <c r="A28" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="17"/>
     </row>
     <row r="29" spans="1:6" ht="51">
-      <c r="A29" s="29"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6" ht="33.950000000000003">
-      <c r="A30" s="29"/>
+    <row r="30" spans="1:6" ht="34">
+      <c r="A30" s="26"/>
       <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" ht="33.950000000000003">
-      <c r="A31" s="29"/>
+    <row r="31" spans="1:6" ht="34">
+      <c r="A31" s="26"/>
       <c r="B31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="33.950000000000003">
-      <c r="A32" s="29"/>
+    <row r="32" spans="1:6" ht="34">
+      <c r="A32" s="26"/>
       <c r="B32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" ht="33.950000000000003">
-      <c r="A33" s="29"/>
+    <row r="33" spans="1:6" ht="34">
+      <c r="A33" s="26"/>
       <c r="B33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" ht="33.950000000000003">
-      <c r="A34" s="29"/>
+    <row r="34" spans="1:6" ht="34">
+      <c r="A34" s="26"/>
       <c r="B34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="33.950000000000003">
-      <c r="A35" s="29"/>
+    <row r="35" spans="1:6" ht="34">
+      <c r="A35" s="26"/>
       <c r="B35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" ht="33.950000000000003">
-      <c r="A36" s="29"/>
+    <row r="36" spans="1:6" ht="34">
+      <c r="A36" s="26"/>
       <c r="B36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D36" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" ht="33.950000000000003">
-      <c r="A37" s="29"/>
+    <row r="37" spans="1:6" ht="34">
+      <c r="A37" s="26"/>
       <c r="B37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="33.950000000000003">
-      <c r="A38" s="29"/>
+    <row r="38" spans="1:6" ht="34">
+      <c r="A38" s="26"/>
       <c r="B38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" ht="33.950000000000003">
-      <c r="A39" s="29"/>
+    <row r="39" spans="1:6" ht="34">
+      <c r="A39" s="26"/>
       <c r="B39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="33.950000000000003">
-      <c r="A40" s="30"/>
+    <row r="40" spans="1:6" ht="34">
+      <c r="A40" s="27"/>
       <c r="B40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D40" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" ht="18.95">
-      <c r="A41" s="31" t="s">
+    <row r="41" spans="1:6" ht="19">
+      <c r="A41" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="D41" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" ht="33.950000000000003">
-      <c r="A42" s="29"/>
+    <row r="42" spans="1:6" ht="34">
+      <c r="A42" s="26"/>
       <c r="B42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" ht="33.950000000000003">
-      <c r="A43" s="29"/>
+    <row r="43" spans="1:6" ht="34">
+      <c r="A43" s="26"/>
       <c r="B43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="D43" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" ht="33.950000000000003">
-      <c r="A44" s="29"/>
+    <row r="44" spans="1:6" ht="34">
+      <c r="A44" s="26"/>
       <c r="B44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="17"/>
     </row>
-    <row r="45" spans="1:6" ht="33.950000000000003">
-      <c r="A45" s="29"/>
+    <row r="45" spans="1:6" ht="34">
+      <c r="A45" s="26"/>
       <c r="B45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" ht="33.950000000000003">
-      <c r="A46" s="29"/>
+    <row r="46" spans="1:6" ht="34">
+      <c r="A46" s="26"/>
       <c r="B46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="17"/>
     </row>
     <row r="47" spans="1:6" ht="51">
-      <c r="A47" s="29"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" ht="33.950000000000003">
-      <c r="A48" s="30"/>
+    <row r="48" spans="1:6" ht="34">
+      <c r="A48" s="27"/>
       <c r="B48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" ht="18.95">
-      <c r="A49" s="31" t="s">
+    <row r="49" spans="1:6" ht="19">
+      <c r="A49" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:6" ht="18.95">
-      <c r="A50" s="30"/>
+    <row r="50" spans="1:6" ht="19">
+      <c r="A50" s="27"/>
       <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="D50" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="17"/>
     </row>
-    <row r="51" spans="1:6" ht="33.950000000000003">
-      <c r="A51" s="31" t="s">
+    <row r="51" spans="1:6" ht="34">
+      <c r="A51" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="E51" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="F51" s="17"/>
+    </row>
+    <row r="52" spans="1:6" ht="34">
+      <c r="A52" s="26"/>
+      <c r="B52" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F51" s="17"/>
-    </row>
-    <row r="52" spans="1:6" ht="33.950000000000003">
-      <c r="A52" s="29"/>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="D52" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="17"/>
     </row>
-    <row r="53" spans="1:6" ht="33.950000000000003">
-      <c r="A53" s="29"/>
+    <row r="53" spans="1:6" ht="34">
+      <c r="A53" s="26"/>
       <c r="B53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="D53" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="17"/>
     </row>
-    <row r="54" spans="1:6" ht="33.950000000000003">
-      <c r="A54" s="29"/>
+    <row r="54" spans="1:6" ht="34">
+      <c r="A54" s="26"/>
       <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D54" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E54" s="11"/>
       <c r="F54" s="17"/>
     </row>
-    <row r="55" spans="1:6" ht="33.950000000000003">
-      <c r="A55" s="30"/>
+    <row r="55" spans="1:6" ht="34">
+      <c r="A55" s="27"/>
       <c r="B55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="D55" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E55" s="11"/>
       <c r="F55" s="17"/>
     </row>
-    <row r="56" spans="1:6" ht="18.95">
-      <c r="A56" s="31" t="s">
+    <row r="56" spans="1:6" ht="19">
+      <c r="A56" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="D56" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" ht="33.950000000000003">
-      <c r="A57" s="29"/>
+    <row r="57" spans="1:6" ht="34">
+      <c r="A57" s="26"/>
       <c r="B57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E57" s="11" t="s">
+      <c r="F57" s="17"/>
+    </row>
+    <row r="58" spans="1:6" ht="19">
+      <c r="A58" s="26"/>
+      <c r="B58" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F57" s="17"/>
-    </row>
-    <row r="58" spans="1:6" ht="18.95">
-      <c r="A58" s="29"/>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D58" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E58" s="11"/>
       <c r="F58" s="17"/>
     </row>
-    <row r="59" spans="1:6" ht="33.950000000000003">
-      <c r="A59" s="29"/>
+    <row r="59" spans="1:6" ht="34">
+      <c r="A59" s="26"/>
       <c r="B59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="D59" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="17"/>
     </row>
-    <row r="60" spans="1:6" ht="18.95">
-      <c r="A60" s="29"/>
+    <row r="60" spans="1:6" ht="19">
+      <c r="A60" s="26"/>
       <c r="B60" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="D60" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E60" s="11"/>
       <c r="F60" s="17"/>
     </row>
-    <row r="61" spans="1:6" ht="18.95">
-      <c r="A61" s="29"/>
+    <row r="61" spans="1:6" ht="19">
+      <c r="A61" s="26"/>
       <c r="B61" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="D61" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="17"/>
     </row>
-    <row r="62" spans="1:6" ht="33.950000000000003">
-      <c r="A62" s="29"/>
+    <row r="62" spans="1:6" ht="34">
+      <c r="A62" s="26"/>
       <c r="B62" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="D62" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="17"/>
     </row>
-    <row r="63" spans="1:6" ht="33.950000000000003">
-      <c r="A63" s="29"/>
+    <row r="63" spans="1:6" ht="34">
+      <c r="A63" s="26"/>
       <c r="B63" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="17"/>
     </row>
-    <row r="64" spans="1:6" ht="33.950000000000003">
-      <c r="A64" s="29"/>
+    <row r="64" spans="1:6" ht="34">
+      <c r="A64" s="26"/>
       <c r="B64" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="D64" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E64" s="11"/>
       <c r="F64" s="17"/>
     </row>
-    <row r="65" spans="1:6" ht="33.950000000000003">
-      <c r="A65" s="30"/>
+    <row r="65" spans="1:6" ht="34">
+      <c r="A65" s="27"/>
       <c r="B65" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D65" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="17"/>
     </row>
-    <row r="66" spans="1:6" ht="61.5">
-      <c r="A66" s="31" t="s">
+    <row r="66" spans="1:6" ht="68">
+      <c r="A66" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E66" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E66" s="11" t="s">
+      <c r="F66" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F66" s="40" t="s">
+    </row>
+    <row r="67" spans="1:6" ht="34">
+      <c r="A67" s="26"/>
+      <c r="B67" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="33.950000000000003">
-      <c r="A67" s="29"/>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="D67" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="17"/>
     </row>
-    <row r="68" spans="1:6" ht="399.75">
-      <c r="A68" s="29"/>
+    <row r="68" spans="1:6" ht="409.6">
+      <c r="A68" s="26"/>
       <c r="B68" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="D68" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E68" s="11" t="s">
+      <c r="F68" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="F68" s="40" t="s">
+    </row>
+    <row r="69" spans="1:6" ht="34">
+      <c r="A69" s="27"/>
+      <c r="B69" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="33.950000000000003">
-      <c r="A69" s="30"/>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="D69" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="17"/>
     </row>
     <row r="70" spans="1:6" ht="51">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E70" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E70" s="11" t="s">
+      <c r="F70" s="17"/>
+    </row>
+    <row r="71" spans="1:6" ht="34">
+      <c r="A71" s="26"/>
+      <c r="B71" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F70" s="17"/>
-    </row>
-    <row r="71" spans="1:6" ht="33.950000000000003">
-      <c r="A71" s="29"/>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="D71" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E71" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E71" s="11" t="s">
+      <c r="F71" s="17"/>
+    </row>
+    <row r="72" spans="1:6" ht="34">
+      <c r="A72" s="26"/>
+      <c r="B72" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F71" s="17"/>
-    </row>
-    <row r="72" spans="1:6" ht="33.950000000000003">
-      <c r="A72" s="29"/>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D72" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E72" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E72" s="11" t="s">
+      <c r="F72" s="17"/>
+    </row>
+    <row r="73" spans="1:6" ht="51">
+      <c r="A73" s="26"/>
+      <c r="B73" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F72" s="17"/>
-    </row>
-    <row r="73" spans="1:6" ht="51">
-      <c r="A73" s="29"/>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="D73" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E73" s="11" t="s">
+      <c r="F73" s="17"/>
+    </row>
+    <row r="74" spans="1:6" ht="34">
+      <c r="A74" s="26"/>
+      <c r="B74" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F73" s="17"/>
-    </row>
-    <row r="74" spans="1:6" ht="33.950000000000003">
-      <c r="A74" s="29"/>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="D74" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E74" s="11"/>
       <c r="F74" s="17"/>
     </row>
-    <row r="75" spans="1:6" ht="33.950000000000003">
-      <c r="A75" s="29"/>
+    <row r="75" spans="1:6" ht="34">
+      <c r="A75" s="26"/>
       <c r="B75" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="D75" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E75" s="11"/>
       <c r="F75" s="17"/>
     </row>
-    <row r="76" spans="1:6" ht="33.950000000000003">
-      <c r="A76" s="29"/>
+    <row r="76" spans="1:6" ht="34">
+      <c r="A76" s="26"/>
       <c r="B76" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="D76" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E76" s="11"/>
       <c r="F76" s="17"/>
     </row>
-    <row r="77" spans="1:6" ht="33.950000000000003">
-      <c r="A77" s="29"/>
+    <row r="77" spans="1:6" ht="34">
+      <c r="A77" s="26"/>
       <c r="B77" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="D77" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="17"/>
     </row>
     <row r="78" spans="1:6" ht="51">
-      <c r="A78" s="29"/>
+      <c r="A78" s="26"/>
       <c r="B78" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="D78" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E78" s="11"/>
       <c r="F78" s="17"/>
     </row>
     <row r="79" spans="1:6" ht="51">
-      <c r="A79" s="29"/>
+      <c r="A79" s="26"/>
       <c r="B79" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C79" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="D79" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="17"/>
     </row>
-    <row r="80" spans="1:6" ht="84.95">
-      <c r="A80" s="29"/>
+    <row r="80" spans="1:6" ht="85">
+      <c r="A80" s="26"/>
       <c r="B80" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="D80" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E80" s="11" t="s">
+      <c r="F80" s="17"/>
+    </row>
+    <row r="81" spans="1:6" ht="51">
+      <c r="A81" s="26"/>
+      <c r="B81" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F80" s="17"/>
-    </row>
-    <row r="81" spans="1:6" ht="51">
-      <c r="A81" s="29"/>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="D81" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F81" s="17"/>
+    </row>
+    <row r="82" spans="1:6" ht="51">
+      <c r="A82" s="26"/>
+      <c r="B82" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D81" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F81" s="17"/>
-    </row>
-    <row r="82" spans="1:6" ht="51">
-      <c r="A82" s="29"/>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="D82" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E82" s="11"/>
       <c r="F82" s="17"/>
     </row>
     <row r="83" spans="1:6" ht="51">
-      <c r="A83" s="30"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="D83" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" ht="18.95">
-      <c r="A84" s="31" t="s">
+    <row r="84" spans="1:6" ht="19">
+      <c r="A84" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="D84" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E84" s="11"/>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" ht="33.950000000000003">
-      <c r="A85" s="29"/>
+    <row r="85" spans="1:6" ht="34">
+      <c r="A85" s="26"/>
       <c r="B85" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="D85" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="17"/>
     </row>
     <row r="86" spans="1:6" ht="51">
-      <c r="A86" s="29"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C86" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="D86" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E86" s="11"/>
       <c r="F86" s="17"/>
     </row>
-    <row r="87" spans="1:6" ht="33.950000000000003">
-      <c r="A87" s="29"/>
+    <row r="87" spans="1:6" ht="34">
+      <c r="A87" s="26"/>
       <c r="B87" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C87" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="D87" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E87" s="11"/>
       <c r="F87" s="17"/>
     </row>
-    <row r="88" spans="1:6" ht="33.950000000000003">
-      <c r="A88" s="29"/>
+    <row r="88" spans="1:6" ht="34">
+      <c r="A88" s="26"/>
       <c r="B88" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>195</v>
-      </c>
       <c r="D88" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E88" s="11"/>
       <c r="F88" s="17"/>
     </row>
-    <row r="89" spans="1:6" ht="33.950000000000003">
-      <c r="A89" s="29"/>
+    <row r="89" spans="1:6" ht="34">
+      <c r="A89" s="26"/>
       <c r="B89" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="D89" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E89" s="11"/>
       <c r="F89" s="17"/>
     </row>
-    <row r="90" spans="1:6" ht="33.950000000000003">
-      <c r="A90" s="29"/>
+    <row r="90" spans="1:6" ht="34">
+      <c r="A90" s="26"/>
       <c r="B90" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="D90" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E90" s="11"/>
       <c r="F90" s="17"/>
     </row>
-    <row r="91" spans="1:6" ht="33.950000000000003">
-      <c r="A91" s="29"/>
+    <row r="91" spans="1:6" ht="34">
+      <c r="A91" s="26"/>
       <c r="B91" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="D91" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E91" s="11"/>
       <c r="F91" s="17"/>
     </row>
-    <row r="92" spans="1:6" ht="33.950000000000003">
-      <c r="A92" s="29"/>
+    <row r="92" spans="1:6" ht="34">
+      <c r="A92" s="26"/>
       <c r="B92" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="D92" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E92" s="11"/>
       <c r="F92" s="17"/>
     </row>
-    <row r="93" spans="1:6" ht="33.950000000000003">
-      <c r="A93" s="29"/>
+    <row r="93" spans="1:6" ht="34">
+      <c r="A93" s="26"/>
       <c r="B93" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="D93" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E93" s="11"/>
       <c r="F93" s="17"/>
     </row>
     <row r="94" spans="1:6" ht="51">
-      <c r="A94" s="29"/>
+      <c r="A94" s="26"/>
       <c r="B94" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="D94" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E94" s="11"/>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:6" ht="84.95">
-      <c r="A95" s="29"/>
+    <row r="95" spans="1:6" ht="85">
+      <c r="A95" s="26"/>
       <c r="B95" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="D95" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E95" s="11"/>
       <c r="F95" s="17"/>
     </row>
     <row r="96" spans="1:6" ht="51">
-      <c r="A96" s="30"/>
+      <c r="A96" s="27"/>
       <c r="B96" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="D96" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E96" s="11"/>
       <c r="F96" s="17"/>
     </row>
-    <row r="97" spans="1:6" ht="33.950000000000003">
-      <c r="A97" s="31" t="s">
+    <row r="97" spans="1:6" ht="34">
+      <c r="A97" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>214</v>
-      </c>
       <c r="D97" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E97" s="11"/>
       <c r="F97" s="17"/>
     </row>
-    <row r="98" spans="1:6" ht="33.950000000000003">
-      <c r="A98" s="29"/>
+    <row r="98" spans="1:6" ht="34">
+      <c r="A98" s="26"/>
       <c r="B98" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="D98" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E98" s="11"/>
       <c r="F98" s="17"/>
     </row>
-    <row r="99" spans="1:6" ht="18.95">
-      <c r="A99" s="29"/>
+    <row r="99" spans="1:6" ht="19">
+      <c r="A99" s="26"/>
       <c r="B99" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="D99" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E99" s="11"/>
       <c r="F99" s="17"/>
     </row>
-    <row r="100" spans="1:6" ht="33.950000000000003">
-      <c r="A100" s="29"/>
+    <row r="100" spans="1:6" ht="34">
+      <c r="A100" s="26"/>
       <c r="B100" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="D100" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E100" s="11"/>
       <c r="F100" s="17"/>
     </row>
-    <row r="101" spans="1:6" ht="33.950000000000003">
-      <c r="A101" s="29"/>
+    <row r="101" spans="1:6" ht="34">
+      <c r="A101" s="26"/>
       <c r="B101" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C101" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="D101" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E101" s="11"/>
       <c r="F101" s="17"/>
     </row>
-    <row r="102" spans="1:6" ht="68.099999999999994">
-      <c r="A102" s="29"/>
+    <row r="102" spans="1:6" ht="68">
+      <c r="A102" s="26"/>
       <c r="B102" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>224</v>
-      </c>
       <c r="D102" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E102" s="11"/>
       <c r="F102" s="17"/>
     </row>
-    <row r="103" spans="1:6" ht="33.950000000000003">
-      <c r="A103" s="29"/>
+    <row r="103" spans="1:6" ht="34">
+      <c r="A103" s="26"/>
       <c r="B103" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>226</v>
-      </c>
       <c r="D103" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E103" s="11"/>
       <c r="F103" s="17"/>
     </row>
-    <row r="104" spans="1:6" ht="18.95">
-      <c r="A104" s="29"/>
+    <row r="104" spans="1:6" ht="19">
+      <c r="A104" s="26"/>
       <c r="B104" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>228</v>
-      </c>
       <c r="D104" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E104" s="11"/>
       <c r="F104" s="17"/>
     </row>
-    <row r="105" spans="1:6" ht="33.950000000000003">
-      <c r="A105" s="29"/>
+    <row r="105" spans="1:6" ht="34">
+      <c r="A105" s="26"/>
       <c r="B105" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="C105" s="3" t="s">
-        <v>230</v>
-      </c>
       <c r="D105" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E105" s="11"/>
       <c r="F105" s="17"/>
     </row>
     <row r="106" spans="1:6" ht="51">
-      <c r="A106" s="29"/>
+      <c r="A106" s="26"/>
       <c r="B106" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C106" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="D106" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E106" s="11"/>
       <c r="F106" s="17"/>
     </row>
     <row r="107" spans="1:6" ht="51">
-      <c r="A107" s="30"/>
+      <c r="A107" s="27"/>
       <c r="B107" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>234</v>
-      </c>
       <c r="D107" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="17"/>
     </row>
-    <row r="108" spans="1:6" ht="33.950000000000003">
-      <c r="A108" s="31" t="s">
+    <row r="108" spans="1:6" ht="34">
+      <c r="A108" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>237</v>
-      </c>
       <c r="D108" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E108" s="11"/>
       <c r="F108" s="17"/>
     </row>
     <row r="109" spans="1:6" ht="51">
-      <c r="A109" s="29"/>
+      <c r="A109" s="26"/>
       <c r="B109" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C109" s="3" t="s">
-        <v>239</v>
-      </c>
       <c r="D109" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E109" s="11"/>
       <c r="F109" s="17"/>
     </row>
     <row r="110" spans="1:6" ht="51">
-      <c r="A110" s="29"/>
+      <c r="A110" s="26"/>
       <c r="B110" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C110" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="D110" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E110" s="11"/>
       <c r="F110" s="17"/>
     </row>
-    <row r="111" spans="1:6" ht="33.950000000000003">
-      <c r="A111" s="29"/>
+    <row r="111" spans="1:6" ht="34">
+      <c r="A111" s="26"/>
       <c r="B111" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>243</v>
-      </c>
       <c r="D111" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E111" s="11"/>
       <c r="F111" s="17"/>
     </row>
-    <row r="112" spans="1:6" ht="33.950000000000003">
-      <c r="A112" s="29"/>
+    <row r="112" spans="1:6" ht="34">
+      <c r="A112" s="26"/>
       <c r="B112" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>245</v>
-      </c>
       <c r="D112" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E112" s="11"/>
       <c r="F112" s="17"/>
     </row>
     <row r="113" spans="1:6" ht="51">
-      <c r="A113" s="29"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="C113" s="3" t="s">
-        <v>247</v>
-      </c>
       <c r="D113" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E113" s="11"/>
       <c r="F113" s="17"/>
     </row>
-    <row r="114" spans="1:6" ht="33.950000000000003">
-      <c r="A114" s="29"/>
+    <row r="114" spans="1:6" ht="34">
+      <c r="A114" s="26"/>
       <c r="B114" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C114" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="D114" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E114" s="11"/>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:6" ht="33.950000000000003">
-      <c r="A115" s="29"/>
+    <row r="115" spans="1:6" ht="34">
+      <c r="A115" s="26"/>
       <c r="B115" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C115" s="3" t="s">
-        <v>251</v>
-      </c>
       <c r="D115" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E115" s="11"/>
       <c r="F115" s="17"/>
     </row>
     <row r="116" spans="1:6" ht="51">
-      <c r="A116" s="29"/>
+      <c r="A116" s="26"/>
       <c r="B116" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C116" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="D116" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E116" s="11"/>
       <c r="F116" s="17"/>
     </row>
     <row r="117" spans="1:6" ht="51">
-      <c r="A117" s="29"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C117" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="D117" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E117" s="11"/>
       <c r="F117" s="17"/>
     </row>
     <row r="118" spans="1:6" ht="51">
-      <c r="A118" s="29"/>
+      <c r="A118" s="26"/>
       <c r="B118" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C118" s="3" t="s">
-        <v>257</v>
-      </c>
       <c r="D118" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E118" s="11"/>
       <c r="F118" s="17"/>
     </row>
     <row r="119" spans="1:6" ht="51">
-      <c r="A119" s="30"/>
+      <c r="A119" s="27"/>
       <c r="B119" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>259</v>
-      </c>
       <c r="D119" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E119" s="11"/>
       <c r="F119" s="17"/>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="38" t="s">
+      <c r="A123" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="B123" s="37"/>
+      <c r="C123" s="37"/>
+      <c r="D123" s="37"/>
+      <c r="E123" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="B123" s="38"/>
-      <c r="C123" s="38"/>
-      <c r="D123" s="38"/>
-      <c r="E123" s="10" t="s">
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="38" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="39" t="s">
+      <c r="B124" s="38"/>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38"/>
+      <c r="E124" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="B124" s="39"/>
-      <c r="C124" s="39"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="15" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="35"/>
-      <c r="B125" s="36"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="37"/>
+      <c r="A125" s="34"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="35"/>
+      <c r="D125" s="36"/>
       <c r="E125" s="15"/>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="35"/>
-      <c r="B126" s="36"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="37"/>
+      <c r="A126" s="34"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="35"/>
+      <c r="D126" s="36"/>
       <c r="E126" s="15"/>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="32"/>
-      <c r="B127" s="33"/>
-      <c r="C127" s="33"/>
-      <c r="D127" s="34"/>
+      <c r="A127" s="31"/>
+      <c r="B127" s="32"/>
+      <c r="C127" s="32"/>
+      <c r="D127" s="33"/>
       <c r="E127" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A14:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A28:A40"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A127:D127"/>
@@ -3452,19 +3463,6 @@
     <mergeCell ref="A66:A69"/>
     <mergeCell ref="A70:A83"/>
     <mergeCell ref="A84:A96"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A14:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:E119">
     <cfRule type="expression" dxfId="3" priority="1">

</xml_diff>